<commit_message>
Integrating data from Merkel ROC curve
</commit_message>
<xml_diff>
--- a/experimental_data/GEC/Merkel1991.xlsx
+++ b/experimental_data/GEC/Merkel1991.xlsx
@@ -59,22 +59,22 @@
     <t>Predictor [GEC, Pugh]</t>
   </si>
   <si>
+    <t>1-specificity (false positive rate)</t>
+  </si>
+  <si>
     <t>Sensitivity (true positive rate)</t>
   </si>
   <si>
-    <t>1-specificity (false positive rate)</t>
-  </si>
-  <si>
     <t>cutoff</t>
   </si>
   <si>
     <t>predictor</t>
   </si>
   <si>
+    <t>fpr</t>
+  </si>
+  <si>
     <t>tpr</t>
-  </si>
-  <si>
-    <t>fpr</t>
   </si>
   <si>
     <t>mer1991</t>
@@ -335,7 +335,7 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>250920</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>110520</xdr:rowOff>
+      <xdr:rowOff>87840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -374,7 +374,7 @@
   <dimension ref="A1:V29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -436,7 +436,7 @@
     <row r="9" customFormat="false" ht="13.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="5"/>
     </row>
-    <row r="10" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
@@ -479,7 +479,7 @@
         <v>19</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>